<commit_message>
2022-02-22 Orbits, MTG, Motherload
</commit_message>
<xml_diff>
--- a/SQL/Transactions Analysis/pcbanking.xlsx
+++ b/SQL/Transactions Analysis/pcbanking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrig\Documents\Coding_Practice\SQL\Transactions Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFB7E84-6430-474C-8D8D-162C7CA0D5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A054F0-5C30-41C3-AD97-6F7C442DC8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5689" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5713" uniqueCount="490">
   <si>
     <t>-</t>
   </si>
@@ -1493,12 +1493,21 @@
   </si>
   <si>
     <t>FPOS CARLETON CO-OP COUNTFLORE</t>
+  </si>
+  <si>
+    <t>OPOS 128.97 FRG*NBASTORE.JACKS</t>
+  </si>
+  <si>
+    <t>OPOS 128.97 FRG*NBASTORE.86674</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1976,10 +1985,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2335,10 +2345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1945"/>
+  <dimension ref="A1:F1953"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1936" workbookViewId="0">
-      <selection activeCell="F1946" sqref="F1946"/>
+    <sheetView tabSelected="1" topLeftCell="A1939" workbookViewId="0">
+      <selection activeCell="D1953" sqref="D1953"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39637,6 +39647,142 @@
         <v>25</v>
       </c>
     </row>
+    <row r="1946" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1946" s="3">
+        <v>44609</v>
+      </c>
+      <c r="B1946">
+        <v>-38.99</v>
+      </c>
+      <c r="C1946" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1946" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1946" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1947" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1947" s="3">
+        <v>44608</v>
+      </c>
+      <c r="B1947">
+        <v>-171.73</v>
+      </c>
+      <c r="C1947" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1947" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1947" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="1948" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1948" s="3">
+        <v>44603</v>
+      </c>
+      <c r="B1948">
+        <v>159.27000000000001</v>
+      </c>
+      <c r="C1948" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1948" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1948" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="1949" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1949" s="3">
+        <v>44603</v>
+      </c>
+      <c r="B1949">
+        <v>-29.99</v>
+      </c>
+      <c r="C1949" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1949" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1949" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1950" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1950" s="3">
+        <v>44603</v>
+      </c>
+      <c r="B1950">
+        <v>-33.340000000000003</v>
+      </c>
+      <c r="C1950" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1950" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1950" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1951" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1951" s="3">
+        <v>44603</v>
+      </c>
+      <c r="B1951">
+        <v>-94.11</v>
+      </c>
+      <c r="C1951" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1951" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1951" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1952" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1952" s="3">
+        <v>44603</v>
+      </c>
+      <c r="B1952">
+        <v>-168.29</v>
+      </c>
+      <c r="C1952" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1952" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1952" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="1953" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1953" s="2">
+        <v>44610</v>
+      </c>
+      <c r="B1953">
+        <v>-65.819999999999993</v>
+      </c>
+      <c r="C1953" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1953" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1953" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2022-03-13 Who Pays Who Java
</commit_message>
<xml_diff>
--- a/SQL/Transactions Analysis/pcbanking.xlsx
+++ b/SQL/Transactions Analysis/pcbanking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrig\Documents\Coding_Practice\SQL\Transactions Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D5338D-3F97-4E7B-838E-22BAB38B8B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF6A8D6-2C2A-46A7-9344-3B999ABEC7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5734" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5755" uniqueCount="496">
   <si>
     <t>-</t>
   </si>
@@ -1502,6 +1502,21 @@
   </si>
   <si>
     <t>OPOS NEWEGG CANADA INC   RICHM</t>
+  </si>
+  <si>
+    <t>OPOS Starlink Internet   Halifax      CA</t>
+  </si>
+  <si>
+    <t>DEPOSIT</t>
+  </si>
+  <si>
+    <t>FPOS SMITH DRUGS         FLORENCEVILNBCA</t>
+  </si>
+  <si>
+    <t>FPOS TIM HORTONS #2853   BRISTOL    NBCD</t>
+  </si>
+  <si>
+    <t>FPOS ULTRAMAR #12659     BATH      NBCA</t>
   </si>
 </sst>
 </file>
@@ -2348,10 +2363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1960"/>
+  <dimension ref="A1:F1967"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1939" workbookViewId="0">
-      <selection activeCell="A1960" sqref="A1960"/>
+    <sheetView tabSelected="1" topLeftCell="A1936" workbookViewId="0">
+      <selection activeCell="A1968" sqref="A1968"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39905,6 +39920,125 @@
         <v>12</v>
       </c>
     </row>
+    <row r="1961" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1961" s="2">
+        <v>44631</v>
+      </c>
+      <c r="B1961">
+        <v>-100.75</v>
+      </c>
+      <c r="C1961" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1961" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1961" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1962" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1962" s="2">
+        <v>44631</v>
+      </c>
+      <c r="B1962">
+        <v>-692.1</v>
+      </c>
+      <c r="C1962" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1962" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1962" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="1963" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1963" s="2">
+        <v>44630</v>
+      </c>
+      <c r="B1963">
+        <v>190</v>
+      </c>
+      <c r="C1963" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1963" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1963" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1964" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1964" s="2">
+        <v>44630</v>
+      </c>
+      <c r="B1964">
+        <v>-27.73</v>
+      </c>
+      <c r="C1964" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1964" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1964" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="1965" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1965" s="2">
+        <v>44630</v>
+      </c>
+      <c r="B1965">
+        <v>-2.0699999999999998</v>
+      </c>
+      <c r="C1965" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1965" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1965" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="1966" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1966" s="2">
+        <v>44630</v>
+      </c>
+      <c r="B1966">
+        <v>1276.24</v>
+      </c>
+      <c r="C1966" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1966" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1966" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1967" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1967" s="2">
+        <v>44628</v>
+      </c>
+      <c r="B1967">
+        <v>-38.270000000000003</v>
+      </c>
+      <c r="C1967" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1967" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1967" t="s">
+        <v>495</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2022-03-16 Who Pays Who
</commit_message>
<xml_diff>
--- a/SQL/Transactions Analysis/pcbanking.xlsx
+++ b/SQL/Transactions Analysis/pcbanking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrig\Documents\Coding_Practice\SQL\Transactions Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF6A8D6-2C2A-46A7-9344-3B999ABEC7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39B0337-ED55-4995-9BF9-61A0FD85400A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5755" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5764" uniqueCount="496">
   <si>
     <t>-</t>
   </si>
@@ -2363,10 +2363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1967"/>
+  <dimension ref="A1:F1970"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1936" workbookViewId="0">
-      <selection activeCell="A1968" sqref="A1968"/>
+      <selection activeCell="B1968" sqref="B1968"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40039,6 +40039,57 @@
         <v>495</v>
       </c>
     </row>
+    <row r="1968" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1968" s="2">
+        <v>44634</v>
+      </c>
+      <c r="B1968">
+        <v>-150</v>
+      </c>
+      <c r="C1968" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1968" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1968" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1969" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1969" s="2">
+        <v>44634</v>
+      </c>
+      <c r="B1969">
+        <v>-18.39</v>
+      </c>
+      <c r="C1969" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1969" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1969" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="1970" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1970" s="2">
+        <v>44634</v>
+      </c>
+      <c r="B1970">
+        <v>-120.74</v>
+      </c>
+      <c r="C1970" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1970" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1970" t="s">
+        <v>490</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2022-07-11 Bad Widgets - OrbitingDatePicker
</commit_message>
<xml_diff>
--- a/SQL/Transactions Analysis/pcbanking.xlsx
+++ b/SQL/Transactions Analysis/pcbanking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrig\Documents\Coding_Practice\SQL\Transactions Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B86295A-79D7-425B-8561-34FE81095BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1267F3F7-5DA0-47BA-AE91-6F2C677E2A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="15990" windowHeight="24840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5941" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6077" uniqueCount="513">
   <si>
     <t>-</t>
   </si>
@@ -1547,6 +1547,27 @@
   </si>
   <si>
     <t>FPOS SMITH DRUGS LTD.    FLORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRD. Card Bill Payment </t>
+  </si>
+  <si>
+    <t>CBSA/ASFC PORT OF WOOD   BELLE</t>
+  </si>
+  <si>
+    <t>CNB #021                 WOODS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ULTRAMAR #12659          BATH </t>
+  </si>
+  <si>
+    <t>TIM HORTONS #0931        ELMSD</t>
+  </si>
+  <si>
+    <t>GCDS625 BRISTOL          BRIST</t>
+  </si>
+  <si>
+    <t>OPOS AMZ*Terramar Sports WWW.A</t>
   </si>
 </sst>
 </file>
@@ -2393,10 +2414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2029"/>
+  <dimension ref="A1:F2075"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1984" workbookViewId="0">
-      <selection activeCell="E1999" sqref="E1999"/>
+    <sheetView tabSelected="1" topLeftCell="A2015" workbookViewId="0">
+      <selection activeCell="A2076" sqref="A2076"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41123,6 +41144,782 @@
         <v>94</v>
       </c>
     </row>
+    <row r="2030" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2030" s="2">
+        <v>44712</v>
+      </c>
+      <c r="B2030">
+        <v>-600</v>
+      </c>
+      <c r="C2030" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2030" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2030" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2031" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2031" s="3">
+        <v>44713</v>
+      </c>
+      <c r="B2031">
+        <v>-161</v>
+      </c>
+      <c r="C2031" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2031" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2031" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2032" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2032" s="3">
+        <v>44714</v>
+      </c>
+      <c r="B2032">
+        <v>1276.24</v>
+      </c>
+      <c r="C2032" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2032" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2032" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2033" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2033" s="3">
+        <v>44718</v>
+      </c>
+      <c r="B2033">
+        <v>-4.91</v>
+      </c>
+      <c r="C2033" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2033" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2033" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2034" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2034" s="3">
+        <v>44718</v>
+      </c>
+      <c r="B2034">
+        <v>-113.85</v>
+      </c>
+      <c r="C2034" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2034" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2034" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2035" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2035" s="3">
+        <v>44720</v>
+      </c>
+      <c r="B2035">
+        <v>-33.090000000000003</v>
+      </c>
+      <c r="C2035" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2035" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="2036" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2036" s="3">
+        <v>44720</v>
+      </c>
+      <c r="B2036">
+        <v>944.15</v>
+      </c>
+      <c r="C2036" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2036" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2036" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2037" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2037" s="3">
+        <v>44721</v>
+      </c>
+      <c r="B2037">
+        <v>-24.14</v>
+      </c>
+      <c r="C2037" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2037" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2037" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2038" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2038" s="3">
+        <v>44722</v>
+      </c>
+      <c r="B2038">
+        <v>-47.14</v>
+      </c>
+      <c r="C2038" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2038" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2038" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2039" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2039" s="3">
+        <v>44722</v>
+      </c>
+      <c r="B2039">
+        <v>-29.89</v>
+      </c>
+      <c r="C2039" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2039" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2039" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2040" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2040" s="3">
+        <v>44722</v>
+      </c>
+      <c r="B2040">
+        <v>-68.98</v>
+      </c>
+      <c r="C2040" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2040" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2040" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2041" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2041" s="3">
+        <v>44722</v>
+      </c>
+      <c r="B2041">
+        <v>-72.260000000000005</v>
+      </c>
+      <c r="C2041" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2041" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2041" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2042" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2042" s="3">
+        <v>44722</v>
+      </c>
+      <c r="B2042">
+        <v>-24.14</v>
+      </c>
+      <c r="C2042" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2042" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2042" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2043" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2043" s="3">
+        <v>44725</v>
+      </c>
+      <c r="B2043">
+        <v>-39.03</v>
+      </c>
+      <c r="C2043" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2043" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2043" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2044" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2044" s="3">
+        <v>44728</v>
+      </c>
+      <c r="B2044">
+        <v>1276.24</v>
+      </c>
+      <c r="C2044" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2044" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2044" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2045" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2045" s="3">
+        <v>44729</v>
+      </c>
+      <c r="B2045">
+        <v>-179.96</v>
+      </c>
+      <c r="C2045" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2045" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2045" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2046" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2046" s="3">
+        <v>44729</v>
+      </c>
+      <c r="B2046">
+        <v>-150.04</v>
+      </c>
+      <c r="C2046" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2046" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2046" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2047" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2047" s="3">
+        <v>44732</v>
+      </c>
+      <c r="B2047">
+        <v>-35.64</v>
+      </c>
+      <c r="C2047" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2047" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2047" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2048" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2048" s="3">
+        <v>44732</v>
+      </c>
+      <c r="B2048">
+        <v>35.65</v>
+      </c>
+      <c r="C2048" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2048" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2048" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2049" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2049" s="3">
+        <v>44733</v>
+      </c>
+      <c r="B2049">
+        <v>-8.0399999999999991</v>
+      </c>
+      <c r="C2049" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2049" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2049" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2050" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2050" s="3">
+        <v>44734</v>
+      </c>
+      <c r="B2050">
+        <v>-7.45</v>
+      </c>
+      <c r="C2050" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2050" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2050" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2051" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2051" s="3">
+        <v>44734</v>
+      </c>
+      <c r="B2051">
+        <v>-27.99</v>
+      </c>
+      <c r="C2051" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2051" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2051" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2052" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2052" s="3">
+        <v>44734</v>
+      </c>
+      <c r="B2052">
+        <v>-22.86</v>
+      </c>
+      <c r="C2052" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2052" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2052" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2053" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2053" s="3">
+        <v>44734</v>
+      </c>
+      <c r="B2053">
+        <v>-21.39</v>
+      </c>
+      <c r="C2053" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2053" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2053" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2054" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2054" s="3">
+        <v>44735</v>
+      </c>
+      <c r="B2054">
+        <v>-16.52</v>
+      </c>
+      <c r="C2054" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2054" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2054" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="2055" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2055" s="3">
+        <v>44735</v>
+      </c>
+      <c r="B2055">
+        <v>-90</v>
+      </c>
+      <c r="C2055" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2055" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2055" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2056" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2056" s="3">
+        <v>44735</v>
+      </c>
+      <c r="B2056">
+        <v>-28.49</v>
+      </c>
+      <c r="C2056" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2056" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2056" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="2057" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2057" s="3">
+        <v>44736</v>
+      </c>
+      <c r="B2057">
+        <v>-46.68</v>
+      </c>
+      <c r="C2057" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2057" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2057" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2058" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2058" s="3">
+        <v>44736</v>
+      </c>
+      <c r="B2058">
+        <v>-45.99</v>
+      </c>
+      <c r="C2058" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2058" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2058" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2059" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2059" s="3">
+        <v>44736</v>
+      </c>
+      <c r="B2059">
+        <v>-101.93</v>
+      </c>
+      <c r="C2059" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2059" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2059" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2060" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2060" s="3">
+        <v>44736</v>
+      </c>
+      <c r="B2060">
+        <v>-9.19</v>
+      </c>
+      <c r="C2060" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2060" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2060" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2061" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2061" s="3">
+        <v>44737</v>
+      </c>
+      <c r="B2061">
+        <v>-22.99</v>
+      </c>
+      <c r="C2061" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2061" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2061" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2062" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2062" s="3">
+        <v>44737</v>
+      </c>
+      <c r="B2062">
+        <v>-42.54</v>
+      </c>
+      <c r="C2062" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2062" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2062" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2063" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2063" s="3">
+        <v>44737</v>
+      </c>
+      <c r="B2063">
+        <v>-35.06</v>
+      </c>
+      <c r="C2063" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2063" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2063" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2064" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2064" s="3">
+        <v>44739</v>
+      </c>
+      <c r="B2064">
+        <v>-4.13</v>
+      </c>
+      <c r="C2064" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2064" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2064" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2065" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2065" s="3">
+        <v>44740</v>
+      </c>
+      <c r="B2065">
+        <v>-39.1</v>
+      </c>
+      <c r="C2065" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2065" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2065" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2066" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2066" s="3">
+        <v>44741</v>
+      </c>
+      <c r="B2066">
+        <v>-23.68</v>
+      </c>
+      <c r="C2066" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2066" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2066" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2067" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2067" s="3">
+        <v>44742</v>
+      </c>
+      <c r="B2067">
+        <v>1276.24</v>
+      </c>
+      <c r="C2067" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2067" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2067" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2068" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2068" s="3">
+        <v>44742</v>
+      </c>
+      <c r="B2068">
+        <v>-8.81</v>
+      </c>
+      <c r="C2068" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2068" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2068" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="2069" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2069" s="3">
+        <v>44742</v>
+      </c>
+      <c r="B2069">
+        <v>-600</v>
+      </c>
+      <c r="C2069" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2069" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2069" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2070" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2070" s="3">
+        <v>44744</v>
+      </c>
+      <c r="B2070">
+        <v>-161</v>
+      </c>
+      <c r="C2070" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2070" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2070" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2071" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2071" s="3">
+        <v>44746</v>
+      </c>
+      <c r="B2071">
+        <v>101.93</v>
+      </c>
+      <c r="C2071" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2071" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2071" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="2072" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2072" s="3">
+        <v>44747</v>
+      </c>
+      <c r="B2072">
+        <v>299.04000000000002</v>
+      </c>
+      <c r="C2072" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2072" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2072" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2073" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2073" s="3">
+        <v>44747</v>
+      </c>
+      <c r="B2073">
+        <v>101.93</v>
+      </c>
+      <c r="C2073" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2073" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2073" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="2074" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2074" s="3">
+        <v>44747</v>
+      </c>
+      <c r="B2074">
+        <v>-101.93</v>
+      </c>
+      <c r="C2074" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2074" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2074" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="2075" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2075" s="3">
+        <v>44750</v>
+      </c>
+      <c r="B2075">
+        <v>-696.13</v>
+      </c>
+      <c r="C2075" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2075" t="s">
+        <v>506</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2022-08-08 Catch-up from week off.
</commit_message>
<xml_diff>
--- a/SQL/Transactions Analysis/pcbanking.xlsx
+++ b/SQL/Transactions Analysis/pcbanking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrig\Documents\Coding_Practice\SQL\Transactions Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1267F3F7-5DA0-47BA-AE91-6F2C677E2A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE3FC01-8AA1-415F-B264-3A95A8626BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="15990" windowHeight="24840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6077" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6128" uniqueCount="514">
   <si>
     <t>-</t>
   </si>
@@ -1568,6 +1568,9 @@
   </si>
   <si>
     <t>OPOS AMZ*Terramar Sports WWW.A</t>
+  </si>
+  <si>
+    <t>DR LILLIAN C LINTON PROF FLORE</t>
   </si>
 </sst>
 </file>
@@ -2414,10 +2417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2075"/>
+  <dimension ref="A1:F2092"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2015" workbookViewId="0">
-      <selection activeCell="A2076" sqref="A2076"/>
+    <sheetView tabSelected="1" topLeftCell="A2033" workbookViewId="0">
+      <selection activeCell="E2089" sqref="E2089"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41920,6 +41923,295 @@
         <v>506</v>
       </c>
     </row>
+    <row r="2076" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2076" s="2">
+        <v>44754</v>
+      </c>
+      <c r="B2076">
+        <v>-25.52</v>
+      </c>
+      <c r="C2076" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2076" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2076" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2077" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2077" s="2">
+        <v>44754</v>
+      </c>
+      <c r="B2077">
+        <v>-52.29</v>
+      </c>
+      <c r="C2077" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2077" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2077" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2078" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2078" s="2">
+        <v>44754</v>
+      </c>
+      <c r="B2078">
+        <v>-30</v>
+      </c>
+      <c r="C2078" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2078" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2078" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="2079" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2079" s="2">
+        <v>44755</v>
+      </c>
+      <c r="B2079">
+        <v>-158.79</v>
+      </c>
+      <c r="C2079" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2079" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2079" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2080" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2080" s="2">
+        <v>44755</v>
+      </c>
+      <c r="B2080">
+        <v>-178.18</v>
+      </c>
+      <c r="C2080" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2080" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2080" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2081" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2081" s="2">
+        <v>44755</v>
+      </c>
+      <c r="B2081">
+        <v>-54.03</v>
+      </c>
+      <c r="C2081" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2081" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2081" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2082" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2082" s="2">
+        <v>44755</v>
+      </c>
+      <c r="B2082">
+        <v>-19.54</v>
+      </c>
+      <c r="C2082" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2082" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2082" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2083" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2083" s="2">
+        <v>44755</v>
+      </c>
+      <c r="B2083">
+        <v>-25.75</v>
+      </c>
+      <c r="C2083" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2083" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2083" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2084" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2084" s="2">
+        <v>44755</v>
+      </c>
+      <c r="B2084">
+        <v>-34.4</v>
+      </c>
+      <c r="C2084" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2084" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2084" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2085" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2085" s="2">
+        <v>44756</v>
+      </c>
+      <c r="B2085">
+        <v>1282.53</v>
+      </c>
+      <c r="C2085" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2085" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2085" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2086" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2086" s="2">
+        <v>44756</v>
+      </c>
+      <c r="B2086">
+        <v>-184.77</v>
+      </c>
+      <c r="C2086" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2086" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2086" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2087" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2087" s="2">
+        <v>44756</v>
+      </c>
+      <c r="B2087">
+        <v>-132.96</v>
+      </c>
+      <c r="C2087" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2087" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2087" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2088" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2088" s="2">
+        <v>44757</v>
+      </c>
+      <c r="B2088">
+        <v>-22.99</v>
+      </c>
+      <c r="C2088" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2088" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2088" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2089" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2089" s="2">
+        <v>44764</v>
+      </c>
+      <c r="B2089">
+        <v>-34.44</v>
+      </c>
+      <c r="C2089" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2089" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2089" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2090" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2090" s="2">
+        <v>44769</v>
+      </c>
+      <c r="B2090">
+        <v>-199.99</v>
+      </c>
+      <c r="C2090" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2090" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2090" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2091" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2091" s="2">
+        <v>44769</v>
+      </c>
+      <c r="B2091">
+        <v>-159.99</v>
+      </c>
+      <c r="C2091" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2091" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2091" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2092" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2092" s="2">
+        <v>44770</v>
+      </c>
+      <c r="B2092">
+        <v>1282.53</v>
+      </c>
+      <c r="C2092" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2092" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2092" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2022-10-03 New resource, Transactions Analysis
</commit_message>
<xml_diff>
--- a/SQL/Transactions Analysis/pcbanking.xlsx
+++ b/SQL/Transactions Analysis/pcbanking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrig\Documents\Coding_Practice\SQL\Transactions Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5D6524-E7D3-4296-82C7-71D2D47E4B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44247E4-6F84-492B-8F2B-AEB71971CD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="15990" windowHeight="24840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-11220" windowWidth="15990" windowHeight="24840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pcbanking" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6206" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6266" uniqueCount="517">
   <si>
     <t>-</t>
   </si>
@@ -1571,6 +1571,15 @@
   </si>
   <si>
     <t>DR LILLIAN C LINTON PROF FLORE</t>
+  </si>
+  <si>
+    <t>OPOS GASPARD             WINNI</t>
+  </si>
+  <si>
+    <t>CENTREVILLE VALU FOODS   CENTR</t>
+  </si>
+  <si>
+    <t>MCDONALD'S #17867        WOODS</t>
   </si>
 </sst>
 </file>
@@ -2417,10 +2426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2119"/>
+  <dimension ref="A1:F2140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2084" workbookViewId="0">
-      <selection activeCell="A2120" sqref="A2120"/>
+    <sheetView tabSelected="1" topLeftCell="A2042" workbookViewId="0">
+      <selection activeCell="C2120" sqref="C2120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42662,6 +42671,354 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2120" s="3">
+        <v>44811</v>
+      </c>
+      <c r="B2120">
+        <v>-35.18</v>
+      </c>
+      <c r="C2120" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2120" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2120" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2121" s="3">
+        <v>44811</v>
+      </c>
+      <c r="B2121">
+        <v>-1535.99</v>
+      </c>
+      <c r="C2121" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2121" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="2122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2122" s="3">
+        <v>44812</v>
+      </c>
+      <c r="B2122">
+        <v>-35.159999999999997</v>
+      </c>
+      <c r="C2122" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2122" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2122" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2123" s="3">
+        <v>44812</v>
+      </c>
+      <c r="B2123">
+        <v>1282.53</v>
+      </c>
+      <c r="C2123" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2123" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2123" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2124" s="3">
+        <v>44816</v>
+      </c>
+      <c r="B2124">
+        <v>-57.5</v>
+      </c>
+      <c r="C2124" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2124" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2124" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="2125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2125" s="3">
+        <v>44819</v>
+      </c>
+      <c r="B2125">
+        <v>-20.46</v>
+      </c>
+      <c r="C2125" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2125" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2125" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2126" s="3">
+        <v>44820</v>
+      </c>
+      <c r="B2126">
+        <v>-11.5</v>
+      </c>
+      <c r="C2126" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2126" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2126" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="2127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2127" s="3">
+        <v>44820</v>
+      </c>
+      <c r="B2127">
+        <v>-73.27</v>
+      </c>
+      <c r="C2127" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2127" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2127" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2128" s="3">
+        <v>44823</v>
+      </c>
+      <c r="B2128">
+        <v>-40.46</v>
+      </c>
+      <c r="C2128" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2128" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2128" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2129" s="3">
+        <v>44823</v>
+      </c>
+      <c r="B2129">
+        <v>-5.98</v>
+      </c>
+      <c r="C2129" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2129" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2129" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="2130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2130" s="3">
+        <v>44824</v>
+      </c>
+      <c r="B2130">
+        <v>-72.22</v>
+      </c>
+      <c r="C2130" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2130" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2130" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2131" s="3">
+        <v>44824</v>
+      </c>
+      <c r="B2131">
+        <v>-77.260000000000005</v>
+      </c>
+      <c r="C2131" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2131" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2131" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2132" s="3">
+        <v>44824</v>
+      </c>
+      <c r="B2132">
+        <v>-48.91</v>
+      </c>
+      <c r="C2132" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2132" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2132" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2133" s="3">
+        <v>44826</v>
+      </c>
+      <c r="B2133">
+        <v>1282.53</v>
+      </c>
+      <c r="C2133" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2133" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2133" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2134" s="3">
+        <v>44827</v>
+      </c>
+      <c r="B2134">
+        <v>-400</v>
+      </c>
+      <c r="C2134" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2134" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2135" s="3">
+        <v>44830</v>
+      </c>
+      <c r="B2135">
+        <v>-98.86</v>
+      </c>
+      <c r="C2135" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2135" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2135" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2136" s="3">
+        <v>44830</v>
+      </c>
+      <c r="B2136">
+        <v>-32.25</v>
+      </c>
+      <c r="C2136" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2136" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2136" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="2137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2137" s="3">
+        <v>44831</v>
+      </c>
+      <c r="B2137">
+        <v>-28.75</v>
+      </c>
+      <c r="C2137" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2137" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2137" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2138" s="3">
+        <v>44832</v>
+      </c>
+      <c r="B2138">
+        <v>-82.16</v>
+      </c>
+      <c r="C2138" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2138" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2138" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2139" s="3">
+        <v>44832</v>
+      </c>
+      <c r="B2139">
+        <v>7.78</v>
+      </c>
+      <c r="C2139" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2139" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2139" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2140" s="3">
+        <v>44833</v>
+      </c>
+      <c r="B2140">
+        <v>-400</v>
+      </c>
+      <c r="C2140" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2140" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2023-09-06 SiegeChallenge, FunnelTelephoneNumber, TkinterEvents
</commit_message>
<xml_diff>
--- a/SQL/Transactions Analysis/pcbanking.xlsx
+++ b/SQL/Transactions Analysis/pcbanking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrig\Documents\Coding_Practice\SQL\Transactions Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFD0E11-01B8-45CA-B4E0-35E1CE23CA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E132017A-7AC5-4816-832D-88EDF39A74E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pcbanking" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7049" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7111" uniqueCount="546">
   <si>
     <t>-</t>
   </si>
@@ -2504,10 +2504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2404"/>
+  <dimension ref="A1:F2425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2390" workbookViewId="0">
-      <selection activeCell="G2400" sqref="G2400"/>
+    <sheetView tabSelected="1" topLeftCell="A2396" workbookViewId="0">
+      <selection activeCell="K2407" sqref="K2407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47558,6 +47558,360 @@
         <v>12</v>
       </c>
     </row>
+    <row r="2405" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2405" s="2">
+        <v>45132</v>
+      </c>
+      <c r="B2405">
+        <v>-4.53</v>
+      </c>
+      <c r="C2405" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2405" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2405" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2406" s="2">
+        <v>45132</v>
+      </c>
+      <c r="B2406">
+        <v>-2000</v>
+      </c>
+      <c r="C2406" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2406" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2406" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2407" s="2">
+        <v>45132</v>
+      </c>
+      <c r="B2407">
+        <v>-100</v>
+      </c>
+      <c r="C2407" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2407" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2407" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2408" s="2">
+        <v>45134</v>
+      </c>
+      <c r="B2408">
+        <v>1470.33</v>
+      </c>
+      <c r="C2408" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2408" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2408" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2409" s="2">
+        <v>45138</v>
+      </c>
+      <c r="B2409">
+        <v>-600</v>
+      </c>
+      <c r="C2409" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2409" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2409" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2410" s="2">
+        <v>45148</v>
+      </c>
+      <c r="B2410">
+        <v>-1882.57</v>
+      </c>
+      <c r="C2410" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2410" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2411" s="2">
+        <v>45148</v>
+      </c>
+      <c r="B2411">
+        <v>1470.33</v>
+      </c>
+      <c r="C2411" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2411" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2411" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2412" s="2">
+        <v>45149</v>
+      </c>
+      <c r="B2412">
+        <v>-44.98</v>
+      </c>
+      <c r="C2412" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2412" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2412" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2413" s="2">
+        <v>45149</v>
+      </c>
+      <c r="B2413">
+        <v>-2.36</v>
+      </c>
+      <c r="C2413" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2413" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2413" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2414" s="2">
+        <v>45149</v>
+      </c>
+      <c r="B2414">
+        <v>-135</v>
+      </c>
+      <c r="C2414" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2414" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2414" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2415" s="2">
+        <v>45149</v>
+      </c>
+      <c r="B2415">
+        <v>-200</v>
+      </c>
+      <c r="C2415" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2415" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2415" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2416" s="2">
+        <v>45153</v>
+      </c>
+      <c r="B2416">
+        <v>-2.65</v>
+      </c>
+      <c r="C2416" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2416" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2416" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2417" s="2">
+        <v>45153</v>
+      </c>
+      <c r="B2417">
+        <v>-2.36</v>
+      </c>
+      <c r="C2417" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2417" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2417" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2418" s="2">
+        <v>45159</v>
+      </c>
+      <c r="B2418">
+        <v>200</v>
+      </c>
+      <c r="C2418" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2418" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2418" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2419" s="2">
+        <v>45160</v>
+      </c>
+      <c r="B2419">
+        <v>-2.95</v>
+      </c>
+      <c r="C2419" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2419" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2419" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2420" s="2">
+        <v>45160</v>
+      </c>
+      <c r="B2420">
+        <v>-2.36</v>
+      </c>
+      <c r="C2420" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2420" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2420" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2421" s="2">
+        <v>45162</v>
+      </c>
+      <c r="B2421">
+        <v>1470.33</v>
+      </c>
+      <c r="C2421" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2421" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2421" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2422" s="2">
+        <v>45166</v>
+      </c>
+      <c r="B2422">
+        <v>-34.49</v>
+      </c>
+      <c r="C2422" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2422" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2422" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2423" s="2">
+        <v>45168</v>
+      </c>
+      <c r="B2423">
+        <v>203.26</v>
+      </c>
+      <c r="C2423" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2423" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2423" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2424" s="2">
+        <v>45168</v>
+      </c>
+      <c r="B2424">
+        <v>214</v>
+      </c>
+      <c r="C2424" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2424" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2424" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2425" s="2">
+        <v>45169</v>
+      </c>
+      <c r="B2425">
+        <v>-600</v>
+      </c>
+      <c r="C2425" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2425" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2425" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2023-11-29 NHL Stats, Streamlit
</commit_message>
<xml_diff>
--- a/SQL/Transactions Analysis/pcbanking.xlsx
+++ b/SQL/Transactions Analysis/pcbanking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrig\Documents\Coding_Practice\SQL\Transactions Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E132017A-7AC5-4816-832D-88EDF39A74E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EA5DC0-B284-4636-8AFD-F8C4D98AEBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pcbanking" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7111" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7269" uniqueCount="559">
   <si>
     <t>-</t>
   </si>
@@ -1658,6 +1658,45 @@
   </si>
   <si>
     <t xml:space="preserve">BATH STN MAIN            BATH </t>
+  </si>
+  <si>
+    <t>PC-SCOTIABANK GOLD AMEX CARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPOS ESSO COUCHE-TARD    WEST </t>
+  </si>
+  <si>
+    <t>Climate Action Incentive</t>
+  </si>
+  <si>
+    <t>FPOS TIM HORTONS #0423   FREDE</t>
+  </si>
+  <si>
+    <t>RIVERVIEW HONDA          FREDE</t>
+  </si>
+  <si>
+    <t>DOLLARAMA # 167          WOODS</t>
+  </si>
+  <si>
+    <t>FPOS CENTRE BELL CONCESSIMONTR</t>
+  </si>
+  <si>
+    <t>FPOS STADE SAPUTO - CONCEMONTR</t>
+  </si>
+  <si>
+    <t>FPOS PARC OLYMPIQUE STATIMONTR</t>
+  </si>
+  <si>
+    <t>FPOS DEPANNEUR P.BEDARD &amp;VILLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loans                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HONDA CANADA FINANCE INC.    </t>
+  </si>
+  <si>
+    <t>FPOS TIM HORTONS #2853   FLORE</t>
   </si>
 </sst>
 </file>
@@ -2504,10 +2543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2425"/>
+  <dimension ref="A1:F2478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2396" workbookViewId="0">
-      <selection activeCell="K2407" sqref="K2407"/>
+    <sheetView tabSelected="1" topLeftCell="A2408" workbookViewId="0">
+      <selection activeCell="D2422" sqref="D2422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47912,6 +47951,904 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2426" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2426" s="2">
+        <v>45174</v>
+      </c>
+      <c r="B2426">
+        <v>-29.89</v>
+      </c>
+      <c r="C2426" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2426" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2426" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2427" s="2">
+        <v>45174</v>
+      </c>
+      <c r="B2427">
+        <v>-500</v>
+      </c>
+      <c r="C2427" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2427" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2427" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2428" s="2">
+        <v>45176</v>
+      </c>
+      <c r="B2428">
+        <v>-134.25</v>
+      </c>
+      <c r="C2428" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2428" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="2429" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2429" s="2">
+        <v>45176</v>
+      </c>
+      <c r="B2429">
+        <v>1470.33</v>
+      </c>
+      <c r="C2429" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2429" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2429" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2430" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2430" s="2">
+        <v>45181</v>
+      </c>
+      <c r="B2430">
+        <v>-230</v>
+      </c>
+      <c r="C2430" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2430" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2430" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2431" s="2">
+        <v>45181</v>
+      </c>
+      <c r="B2431">
+        <v>-157</v>
+      </c>
+      <c r="C2431" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2431" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2431" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="2432" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2432" s="2">
+        <v>45189</v>
+      </c>
+      <c r="B2432">
+        <v>-2.36</v>
+      </c>
+      <c r="C2432" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2432" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2432" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="2433" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2433" s="2">
+        <v>45189</v>
+      </c>
+      <c r="B2433">
+        <v>-2.95</v>
+      </c>
+      <c r="C2433" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2433" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2433" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2434" s="2">
+        <v>45189</v>
+      </c>
+      <c r="B2434">
+        <v>-9.19</v>
+      </c>
+      <c r="C2434" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2434" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2434" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2435" s="2">
+        <v>45190</v>
+      </c>
+      <c r="B2435">
+        <v>-34.49</v>
+      </c>
+      <c r="C2435" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2435" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2435" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="2436" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2436" s="2">
+        <v>45190</v>
+      </c>
+      <c r="B2436">
+        <v>1470.33</v>
+      </c>
+      <c r="C2436" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2436" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2436" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2437" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2437" s="2">
+        <v>45194</v>
+      </c>
+      <c r="B2437">
+        <v>-400</v>
+      </c>
+      <c r="C2437" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2437" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2437" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2438" s="2">
+        <v>45198</v>
+      </c>
+      <c r="B2438">
+        <v>-34.49</v>
+      </c>
+      <c r="C2438" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2438" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2438" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="2439" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2439" s="2">
+        <v>45198</v>
+      </c>
+      <c r="B2439">
+        <v>-9.19</v>
+      </c>
+      <c r="C2439" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2439" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2439" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2440" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2440" s="2">
+        <v>45202</v>
+      </c>
+      <c r="B2440">
+        <v>-600</v>
+      </c>
+      <c r="C2440" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2440" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2440" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2441" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2441" s="2">
+        <v>45202</v>
+      </c>
+      <c r="B2441">
+        <v>-1000</v>
+      </c>
+      <c r="C2441" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2441" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2441" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="2442" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2442" s="2">
+        <v>45202</v>
+      </c>
+      <c r="B2442">
+        <v>-1000</v>
+      </c>
+      <c r="C2442" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2442" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2442" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2443" s="2">
+        <v>45203</v>
+      </c>
+      <c r="B2443">
+        <v>-12.52</v>
+      </c>
+      <c r="C2443" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2443" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2443" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2444" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2444" s="2">
+        <v>45203</v>
+      </c>
+      <c r="B2444">
+        <v>-135</v>
+      </c>
+      <c r="C2444" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2444" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2444" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="2445" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2445" s="2">
+        <v>45203</v>
+      </c>
+      <c r="B2445">
+        <v>-215</v>
+      </c>
+      <c r="C2445" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2445" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2445" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2446" s="2">
+        <v>45204</v>
+      </c>
+      <c r="B2446">
+        <v>106.25</v>
+      </c>
+      <c r="C2446" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2446" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2446" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2447" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2447" s="2">
+        <v>45204</v>
+      </c>
+      <c r="B2447">
+        <v>1470.33</v>
+      </c>
+      <c r="C2447" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2447" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2447" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2448" s="2">
+        <v>45205</v>
+      </c>
+      <c r="B2448">
+        <v>-34.49</v>
+      </c>
+      <c r="C2448" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2448" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2448" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2449" s="2">
+        <v>45210</v>
+      </c>
+      <c r="B2449">
+        <v>-5.27</v>
+      </c>
+      <c r="C2449" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2449" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2449" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="2450" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2450" s="2">
+        <v>45210</v>
+      </c>
+      <c r="B2450">
+        <v>-750</v>
+      </c>
+      <c r="C2450" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2450" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2450" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="2451" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2451" s="2">
+        <v>45212</v>
+      </c>
+      <c r="B2451">
+        <v>184</v>
+      </c>
+      <c r="C2451" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2451" t="s">
+        <v>548</v>
+      </c>
+      <c r="E2451" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2452" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2452" s="2">
+        <v>45213</v>
+      </c>
+      <c r="B2452">
+        <v>-2.0699999999999998</v>
+      </c>
+      <c r="C2452" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2452" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2452" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2453" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2453" s="2">
+        <v>45213</v>
+      </c>
+      <c r="B2453">
+        <v>-2.0699999999999998</v>
+      </c>
+      <c r="C2453" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2453" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2453" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="2454" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2454" s="2">
+        <v>45218</v>
+      </c>
+      <c r="B2454">
+        <v>1470.33</v>
+      </c>
+      <c r="C2454" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2454" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2454" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2455" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2455" s="2">
+        <v>45218</v>
+      </c>
+      <c r="B2455">
+        <v>-1000</v>
+      </c>
+      <c r="C2455" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2455" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2455" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="2456" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2456" s="2">
+        <v>45218</v>
+      </c>
+      <c r="B2456">
+        <v>-8000</v>
+      </c>
+      <c r="C2456" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2456" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2456" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="2457" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2457" s="2">
+        <v>45220</v>
+      </c>
+      <c r="B2457">
+        <v>-78.84</v>
+      </c>
+      <c r="C2457" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2457" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2457" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2458" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2458" s="2">
+        <v>45225</v>
+      </c>
+      <c r="B2458">
+        <v>-21.43</v>
+      </c>
+      <c r="C2458" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2458" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2458" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="2459" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2459" s="2">
+        <v>45225</v>
+      </c>
+      <c r="B2459">
+        <v>-100.18</v>
+      </c>
+      <c r="C2459" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2459" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2459" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2460" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2460" s="2">
+        <v>45225</v>
+      </c>
+      <c r="B2460">
+        <v>-19.18</v>
+      </c>
+      <c r="C2460" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2460" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2460" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="2461" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2461" s="2">
+        <v>45225</v>
+      </c>
+      <c r="B2461">
+        <v>-155</v>
+      </c>
+      <c r="C2461" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2461" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2461" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2462" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2462" s="2">
+        <v>45225</v>
+      </c>
+      <c r="B2462">
+        <v>-200</v>
+      </c>
+      <c r="C2462" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2462" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2462" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2463" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2463" s="2">
+        <v>45226</v>
+      </c>
+      <c r="B2463">
+        <v>-2.06</v>
+      </c>
+      <c r="C2463" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2463" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2463" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="2464" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2464" s="2">
+        <v>45227</v>
+      </c>
+      <c r="B2464">
+        <v>-13.25</v>
+      </c>
+      <c r="C2464" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2464" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2464" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="2465" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2465" s="2">
+        <v>45227</v>
+      </c>
+      <c r="B2465">
+        <v>-29.15</v>
+      </c>
+      <c r="C2465" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2465" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2465" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="2466" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2466" s="2">
+        <v>45227</v>
+      </c>
+      <c r="B2466">
+        <v>-7.75</v>
+      </c>
+      <c r="C2466" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2466" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2466" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="2467" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2467" s="2">
+        <v>45227</v>
+      </c>
+      <c r="B2467">
+        <v>-30</v>
+      </c>
+      <c r="C2467" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2467" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2467" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="2468" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2468" s="2">
+        <v>45229</v>
+      </c>
+      <c r="B2468">
+        <v>-8.1</v>
+      </c>
+      <c r="C2468" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2468" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2468" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="2469" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2469" s="2">
+        <v>45230</v>
+      </c>
+      <c r="B2469">
+        <v>-600</v>
+      </c>
+      <c r="C2469" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2469" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2469" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2470" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2470" s="2">
+        <v>45232</v>
+      </c>
+      <c r="B2470">
+        <v>-73.59</v>
+      </c>
+      <c r="C2470" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2470" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2470" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2471" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2471" s="2">
+        <v>45232</v>
+      </c>
+      <c r="B2471">
+        <v>1470.33</v>
+      </c>
+      <c r="C2471" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2471" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2471" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2472" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2472" s="2">
+        <v>45233</v>
+      </c>
+      <c r="B2472">
+        <v>-366.69</v>
+      </c>
+      <c r="C2472" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2472" t="s">
+        <v>556</v>
+      </c>
+      <c r="E2472" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="2473" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2473" s="2">
+        <v>45233</v>
+      </c>
+      <c r="B2473">
+        <v>-214</v>
+      </c>
+      <c r="C2473" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2473" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2473" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2474" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2474" s="2">
+        <v>45233</v>
+      </c>
+      <c r="B2474">
+        <v>-3000</v>
+      </c>
+      <c r="C2474" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2474" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2474" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="2475" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2475" s="2">
+        <v>45238</v>
+      </c>
+      <c r="B2475">
+        <v>-780.37</v>
+      </c>
+      <c r="C2475" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2475" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2475" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="2476" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2476" s="2">
+        <v>45240</v>
+      </c>
+      <c r="B2476">
+        <v>-10.4</v>
+      </c>
+      <c r="C2476" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2476" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2476" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2477" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2477" s="2">
+        <v>45244</v>
+      </c>
+      <c r="B2477">
+        <v>-8.0299999999999994</v>
+      </c>
+      <c r="C2477" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2477" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2477" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="2478" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2478" s="2">
+        <v>45244</v>
+      </c>
+      <c r="B2478">
+        <v>-20.37</v>
+      </c>
+      <c r="C2478" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2478" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2478" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2024-07-02 Hockey Pool, Jerseys
</commit_message>
<xml_diff>
--- a/SQL/Transactions Analysis/pcbanking.xlsx
+++ b/SQL/Transactions Analysis/pcbanking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrig\Documents\Coding_Practice\SQL\Transactions Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65808523-6ECE-404E-B26C-7C4414B9B51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12768A3A-0185-4DA9-AB3C-DC84CBB0E16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-4830" windowWidth="15990" windowHeight="24840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7697" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7747" uniqueCount="573">
   <si>
     <t>-</t>
   </si>
@@ -1733,6 +1733,12 @@
   </si>
   <si>
     <t>FPOS TIM HORTONS #2111   RIVER</t>
+  </si>
+  <si>
+    <t>OPOS Starlink            Halif</t>
+  </si>
+  <si>
+    <t>PC TO 379241652316012</t>
   </si>
 </sst>
 </file>
@@ -2579,10 +2585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2622"/>
+  <dimension ref="A1:F2639"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2570" workbookViewId="0">
-      <selection activeCell="B2622" sqref="B2622:E2622"/>
+    <sheetView tabSelected="1" topLeftCell="A2585" workbookViewId="0">
+      <selection activeCell="B2639" sqref="B2639:F2639"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51321,6 +51327,292 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2623" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2623" s="2">
+        <v>45447</v>
+      </c>
+      <c r="B2623">
+        <v>-155</v>
+      </c>
+      <c r="C2623" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2623" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2623" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2624" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2624" s="2">
+        <v>45450</v>
+      </c>
+      <c r="B2624">
+        <v>-1000</v>
+      </c>
+      <c r="C2624" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2624" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2624" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="2625" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2625" s="2">
+        <v>45450</v>
+      </c>
+      <c r="B2625">
+        <v>-796.91</v>
+      </c>
+      <c r="C2625" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2625" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="2626" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2626" s="2">
+        <v>45450</v>
+      </c>
+      <c r="B2626">
+        <v>25.05</v>
+      </c>
+      <c r="C2626" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2626" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2626" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2627" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2627" s="2">
+        <v>45454</v>
+      </c>
+      <c r="B2627">
+        <v>-161</v>
+      </c>
+      <c r="C2627" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2627" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2627" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="2628" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2628" s="2">
+        <v>45456</v>
+      </c>
+      <c r="B2628">
+        <v>1518.16</v>
+      </c>
+      <c r="C2628" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2628" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2628" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2629" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2629" s="2">
+        <v>45457</v>
+      </c>
+      <c r="B2629">
+        <v>132.1</v>
+      </c>
+      <c r="C2629" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2629" t="s">
+        <v>548</v>
+      </c>
+      <c r="E2629" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2630" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2630" s="2">
+        <v>45457</v>
+      </c>
+      <c r="B2630">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="C2630" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2630" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2630" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2631" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2631" s="2">
+        <v>45457</v>
+      </c>
+      <c r="B2631">
+        <v>-366.69</v>
+      </c>
+      <c r="C2631" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2631" t="s">
+        <v>556</v>
+      </c>
+      <c r="E2631" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="2632" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2632" s="2">
+        <v>45464</v>
+      </c>
+      <c r="B2632">
+        <v>50</v>
+      </c>
+      <c r="C2632" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2632" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2632" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2633" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2633" s="2">
+        <v>45464</v>
+      </c>
+      <c r="B2633">
+        <v>78.58</v>
+      </c>
+      <c r="C2633" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2633" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2633" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2634" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2634" s="2">
+        <v>45467</v>
+      </c>
+      <c r="B2634">
+        <v>-134.31</v>
+      </c>
+      <c r="C2634" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2634" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2634" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="2635" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2635" s="2">
+        <v>45470</v>
+      </c>
+      <c r="B2635">
+        <v>1518.16</v>
+      </c>
+      <c r="C2635" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2635" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2635" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2636" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2636" s="2">
+        <v>45470</v>
+      </c>
+      <c r="B2636">
+        <v>-600</v>
+      </c>
+      <c r="C2636" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2636" t="s">
+        <v>565</v>
+      </c>
+      <c r="E2636" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="2637" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2637" s="2">
+        <v>45471</v>
+      </c>
+      <c r="B2637">
+        <v>-366.69</v>
+      </c>
+      <c r="C2637" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2637" t="s">
+        <v>556</v>
+      </c>
+      <c r="E2637" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="2638" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2638" s="2">
+        <v>45472</v>
+      </c>
+      <c r="B2638">
+        <v>-16.95</v>
+      </c>
+      <c r="C2638" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2638" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2638" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2639" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2639" s="2">
+        <v>45475</v>
+      </c>
+      <c r="B2639">
+        <v>-600</v>
+      </c>
+      <c r="C2639" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2639" t="s">
+        <v>565</v>
+      </c>
+      <c r="E2639" t="s">
+        <v>572</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>